<commit_message>
Adding new code - branch closed
</commit_message>
<xml_diff>
--- a/csse_covid_19_data/nation_wide_data/US_data.xlsx
+++ b/csse_covid_19_data/nation_wide_data/US_data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="US_data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Brazil" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">confirmed_cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed_deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed_recovered</t>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">1/22/20_total</t>
@@ -338,6 +341,72 @@
   </si>
   <si>
     <t xml:space="preserve">5/2/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/3/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/4/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/5/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/6/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/7/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/8/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/9/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/10/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/11/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/12/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/13/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/14/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/15/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/16/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/17/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/18/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/19/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/20/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/21/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/22/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/23/20_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/24/20_total</t>
   </si>
 </sst>
 </file>
@@ -411,12 +480,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E125" activeCellId="0" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -465,1433 +530,2240 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">B2-(C2+D2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">B3-(C3+D3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">B4-(C4+D4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">B5-(C5+D5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">B6-(C6+D6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">B7-(C7+D7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">B8-(C8+D8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">B9-(C9+D9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">B10-(C10+D10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">B11-(C11+D11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">B12-(C12+D12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">B13-(C13+D13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">B14-(C14+D14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">B15-(C15+D15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">B16-(C16+D16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">B17-(C17+D17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">B18-(C18+D18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">B19-(C19+D19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">B20-(C20+D20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">B21-(C21+D21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">B22-(C22+D22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">B23-(C23+D23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">B24-(C24+D24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">B25-(C25+D25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">B26-(C26+D26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">B27-(C27+D27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">B28-(C28+D28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">B29-(C29+D29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">B30-(C30+D30)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">B31-(C31+D31)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">B32-(C32+D32)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">B33-(C33+D33)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">B34-(C34+D34)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">B35-(C35+D35)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">B36-(C36+D36)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <f aca="false">B37-(C37+D37)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">B38-(C38+D38)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">B39-(C39+D39)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">B40-(C40+D40)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">B41-(C41+D41)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">B42-(C42+D42)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">B43-(C43+D43)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">B44-(C44+D44)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>217</v>
+        <v>4</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">B45-(C45+D45)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>262</v>
+        <v>13</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">B46-(C46+D46)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>402</v>
+        <v>13</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">B47-(C47+D47)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>518</v>
+        <v>20</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">B48-(C48+D48)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>583</v>
+        <v>25</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">B49-(C49+D49)</f>
+        <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>959</v>
+        <v>31</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">B50-(C50+D50)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1281</v>
+        <v>38</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">B51-(C51+D51)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>1663</v>
+        <v>52</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">B52-(C52+D52)</f>
+        <v>52</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>2179</v>
+        <v>151</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <f aca="false">B53-(C53+D53)</f>
+        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>2727</v>
+        <v>151</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">B54-(C54+D54)</f>
+        <v>151</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>3499</v>
+        <v>162</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">B55-(C55+D55)</f>
+        <v>162</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>4632</v>
+        <v>200</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">B56-(C56+D56)</f>
+        <v>199</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>6421</v>
+        <v>321</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">B57-(C57+D57)</f>
+        <v>318</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>7783</v>
+        <v>372</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>164</v>
+        <v>3</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>105</v>
+        <v>2</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">B58-(C58+D58)</f>
+        <v>367</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>13747</v>
+        <v>621</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>258</v>
+        <v>6</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>121</v>
+        <v>2</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <f aca="false">B59-(C59+D59)</f>
+        <v>613</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>19273</v>
+        <v>793</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>349</v>
+        <v>11</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>147</v>
+        <v>2</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <f aca="false">B60-(C60+D60)</f>
+        <v>780</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>25600</v>
+        <v>1021</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>176</v>
+        <v>2</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">B61-(C61+D61)</f>
+        <v>1004</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>33276</v>
+        <v>1546</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>586</v>
+        <v>25</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>178</v>
+        <v>2</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">B62-(C62+D62)</f>
+        <v>1519</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>43843</v>
+        <v>1924</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>786</v>
+        <v>34</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>178</v>
+        <v>2</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <f aca="false">B63-(C63+D63)</f>
+        <v>1888</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>53736</v>
+        <v>2247</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>1008</v>
+        <v>46</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>348</v>
+        <v>2</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <f aca="false">B64-(C64+D64)</f>
+        <v>2199</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>65778</v>
+        <v>2554</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>1316</v>
+        <v>59</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>361</v>
+        <v>2</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">B65-(C65+D65)</f>
+        <v>2493</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>83836</v>
+        <v>2985</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>1726</v>
+        <v>77</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>681</v>
+        <v>6</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <f aca="false">B66-(C66+D66)</f>
+        <v>2902</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>101657</v>
+        <v>3417</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>2265</v>
+        <v>92</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>869</v>
+        <v>6</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <f aca="false">B67-(C67+D67)</f>
+        <v>3319</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>121465</v>
+        <v>3904</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>2731</v>
+        <v>111</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>1072</v>
+        <v>6</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <f aca="false">B68-(C68+D68)</f>
+        <v>3787</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>140909</v>
+        <v>4256</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>3420</v>
+        <v>136</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>2665</v>
+        <v>6</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <f aca="false">B69-(C69+D69)</f>
+        <v>4114</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>161831</v>
+        <v>4579</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>4192</v>
+        <v>159</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>5644</v>
+        <v>120</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <f aca="false">B70-(C70+D70)</f>
+        <v>4300</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>188172</v>
+        <v>5717</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>5367</v>
+        <v>201</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>7024</v>
+        <v>127</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <f aca="false">B71-(C71+D71)</f>
+        <v>5389</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>213242</v>
+        <v>6836</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>6501</v>
+        <v>240</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>8474</v>
+        <v>127</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <f aca="false">B72-(C72+D72)</f>
+        <v>6469</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>243622</v>
+        <v>8044</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>7921</v>
+        <v>324</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>9001</v>
+        <v>127</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <f aca="false">B73-(C73+D73)</f>
+        <v>7593</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>275367</v>
+        <v>9056</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>9246</v>
+        <v>359</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>9707</v>
+        <v>127</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <f aca="false">B74-(C74+D74)</f>
+        <v>8570</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>308650</v>
+        <v>10360</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>10855</v>
+        <v>445</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>14652</v>
+        <v>127</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <f aca="false">B75-(C75+D75)</f>
+        <v>9788</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>336802</v>
+        <v>11130</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>12375</v>
+        <v>486</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>17448</v>
+        <v>127</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <f aca="false">B76-(C76+D76)</f>
+        <v>10517</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>366317</v>
+        <v>12161</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>13894</v>
+        <v>564</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>19581</v>
+        <v>127</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <f aca="false">B77-(C77+D77)</f>
+        <v>11470</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>397121</v>
+        <v>14034</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>16191</v>
+        <v>686</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>21763</v>
+        <v>127</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <f aca="false">B78-(C78+D78)</f>
+        <v>13221</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>428654</v>
+        <v>16170</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>18270</v>
+        <v>819</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>23559</v>
+        <v>127</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <f aca="false">B79-(C79+D79)</f>
+        <v>15224</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>462780</v>
+        <v>18092</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>20255</v>
+        <v>950</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>25410</v>
+        <v>173</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <f aca="false">B80-(C80+D80)</f>
+        <v>16969</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>496535</v>
+        <v>19638</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>22333</v>
+        <v>1057</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>28790</v>
+        <v>173</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <f aca="false">B81-(C81+D81)</f>
+        <v>18408</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>526396</v>
+        <v>20727</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>24342</v>
+        <v>1124</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>31270</v>
+        <v>173</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <f aca="false">B82-(C82+D82)</f>
+        <v>19430</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>555313</v>
+        <v>22192</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>26086</v>
+        <v>1223</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>32988</v>
+        <v>173</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <f aca="false">B83-(C83+D83)</f>
+        <v>20796</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>580619</v>
+        <v>23430</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>27870</v>
+        <v>1328</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>43482</v>
+        <v>173</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <f aca="false">B84-(C84+D84)</f>
+        <v>21929</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>607670</v>
+        <v>25262</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>30262</v>
+        <v>1532</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>47763</v>
+        <v>3046</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">B85-(C85+D85)</f>
+        <v>20684</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>636350</v>
+        <v>28320</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>32734</v>
+        <v>1736</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>52096</v>
+        <v>14026</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">B86-(C86+D86)</f>
+        <v>12558</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>667592</v>
+        <v>30425</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>34827</v>
+        <v>1924</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>54703</v>
+        <v>14026</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">B87-(C87+D87)</f>
+        <v>14475</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>699706</v>
+        <v>33682</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>37411</v>
+        <v>2141</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>58545</v>
+        <v>14026</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <f aca="false">B88-(C88+D88)</f>
+        <v>17515</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>732197</v>
+        <v>36658</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>39753</v>
+        <v>2354</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>64840</v>
+        <v>14026</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <f aca="false">B89-(C89+D89)</f>
+        <v>20278</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>758809</v>
+        <v>38654</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>40945</v>
+        <v>2462</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>70337</v>
+        <v>22130</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <f aca="false">B90-(C90+D90)</f>
+        <v>14062</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>784326</v>
+        <v>40743</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>42659</v>
+        <v>2587</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>72329</v>
+        <v>22130</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <f aca="false">B91-(C91+D91)</f>
+        <v>16026</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>811865</v>
+        <v>43079</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>45086</v>
+        <v>2741</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>75204</v>
+        <v>22991</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">B92-(C92+D92)</f>
+        <v>17347</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>840351</v>
+        <v>45757</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>47412</v>
+        <v>2906</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>77366</v>
+        <v>25318</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">B93-(C93+D93)</f>
+        <v>17533</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>869170</v>
+        <v>50036</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>49724</v>
+        <v>3331</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>80203</v>
+        <v>26573</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <f aca="false">B94-(C94+D94)</f>
+        <v>20132</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>905358</v>
+        <v>54043</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>51493</v>
+        <v>3704</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>99079</v>
+        <v>27655</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <f aca="false">B95-(C95+D95)</f>
+        <v>22684</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>938154</v>
+        <v>59324</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>53755</v>
+        <v>4057</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>100372</v>
+        <v>29160</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <f aca="false">B96-(C96+D96)</f>
+        <v>26107</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>965785</v>
+        <v>63100</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>54881</v>
+        <v>4286</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>106988</v>
+        <v>30152</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <f aca="false">B97-(C97+D97)</f>
+        <v>28662</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>988197</v>
+        <v>67446</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>56259</v>
+        <v>4603</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>111424</v>
+        <v>31142</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <f aca="false">B98-(C98+D98)</f>
+        <v>31701</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>1012582</v>
+        <v>73235</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>58355</v>
+        <v>5083</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>115936</v>
+        <v>32544</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <f aca="false">B99-(C99+D99)</f>
+        <v>35608</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>1039909</v>
+        <v>79685</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>60967</v>
+        <v>5513</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>120720</v>
+        <v>34132</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <f aca="false">B100-(C100+D100)</f>
+        <v>40040</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>1069424</v>
+        <v>87187</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>62996</v>
+        <v>6006</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>153947</v>
+        <v>35935</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <f aca="false">B101-(C101+D101)</f>
+        <v>45246</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>1103461</v>
+        <v>92202</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>64943</v>
+        <v>6412</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>164015</v>
+        <v>38039</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <f aca="false">B102-(C102+D102)</f>
+        <v>47751</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>1132539</v>
+        <v>97100</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>66369</v>
+        <v>6761</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>175382</v>
+        <v>40937</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <f aca="false">B103-(C103+D103)</f>
+        <v>49402</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>101826</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>7051</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>42991</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <f aca="false">B104-(C104+D104)</f>
+        <v>51784</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>108620</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>7367</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>45815</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <f aca="false">B105-(C105+D105)</f>
+        <v>55438</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>115455</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>7938</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>48221</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <f aca="false">B106-(C106+D106)</f>
+        <v>59296</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>126611</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>8588</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>51370</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <f aca="false">B107-(C107+D107)</f>
+        <v>66653</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>135773</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>9190</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>55350</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <f aca="false">B108-(C108+D108)</f>
+        <v>71233</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>146894</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>10017</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>59297</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <f aca="false">B109-(C109+D109)</f>
+        <v>77580</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>156061</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>10656</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>61685</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <f aca="false">B110-(C110+D110)</f>
+        <v>83720</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>162699</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>11123</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>64957</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <f aca="false">B111-(C111+D111)</f>
+        <v>86619</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>169594</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>11653</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>67384</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <f aca="false">B112-(C112+D112)</f>
+        <v>90557</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>178214</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>12461</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>72597</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <f aca="false">B113-(C113+D113)</f>
+        <v>93156</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>190137</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>13240</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>78424</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <f aca="false">B114-(C114+D114)</f>
+        <v>98473</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>203165</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>13999</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>79479</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <f aca="false">B115-(C115+D115)</f>
+        <v>109687</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>220291</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>14962</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>84970</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <f aca="false">B116-(C116+D116)</f>
+        <v>120359</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>233511</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>15662</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>89672</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <f aca="false">B117-(C117+D117)</f>
+        <v>128177</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>241080</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>16118</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>94122</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <f aca="false">B118-(C118+D118)</f>
+        <v>130840</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>255368</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>16853</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>100459</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <f aca="false">B119-(C119+D119)</f>
+        <v>138056</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>271885</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>17983</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>106794</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <f aca="false">B120-(C120+D120)</f>
+        <v>147108</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>291579</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>18859</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>116683</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <f aca="false">B121-(C121+D121)</f>
+        <v>156037</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>310087</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>20047</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>125960</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <f aca="false">B122-(C122+D122)</f>
+        <v>164080</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>330890</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>21048</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>135430</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <f aca="false">B123-(C123+D123)</f>
+        <v>174412</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>347398</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>22013</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>142587</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <f aca="false">B124-(C124+D124)</f>
+        <v>182798</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>363211</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>22666</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>149911</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <f aca="false">B125-(C125+D125)</f>
+        <v>190634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>